<commit_message>
handle errors in formula cells
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/with_errors_all_types.xlsx
+++ b/src/test/resources/spreadsheets/with_errors_all_types.xlsx
@@ -1,17 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\anylyze\forks\spark-excel\src\test\resources\spreadsheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09331708-A9B5-49DA-A531-2E6D64BD639B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="5595" yWindow="2535" windowWidth="20670" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>double</t>
   </si>
@@ -26,23 +69,26 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>formula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -51,11 +97,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -69,38 +121,42 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -290,23 +346,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="13.75"/>
+    <col min="1" max="4" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -319,36 +377,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>44246.0</v>
+        <v>44246</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="2" t="str">
+        <f>_xlfn.CONCAT("A", 3/3)</f>
+        <v>A1</v>
+      </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="3">
-        <v>44246.0</v>
+        <v>44246</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="2" t="str">
+        <f>_xlfn.CONCAT("A", 3/1)</f>
+        <v>A3</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="e">
         <v>#NULL!</v>
       </c>
@@ -361,8 +430,12 @@
       <c r="D4" s="2" t="e">
         <v>#NULL!</v>
       </c>
+      <c r="E4" s="2" t="e">
+        <f>_xlfn.CONCAT("A", 3/0)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="e">
         <v>#N/A</v>
       </c>
@@ -375,11 +448,13 @@
       <c r="D5" s="2" t="e">
         <v>#N/A</v>
       </c>
+      <c r="E5" s="2" t="e" cm="1">
+        <f t="array" ref="E5">NA</f>
+        <v>#NAME?</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>